<commit_message>
add some controllers, update api-map
</commit_message>
<xml_diff>
--- a/api_map.xlsx
+++ b/api_map.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksandr_Sakhnenko\IdeaProjects\epam-lab-spring-evernote\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victor_chuprakov\IdeaProjects\epam-lab-spring-evernote\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>URL path</t>
   </si>
@@ -78,12 +78,18 @@
   </si>
   <si>
     <t>Получение всех заметок с таким тегом</t>
+  </si>
+  <si>
+    <t>logout page</t>
+  </si>
+  <si>
+    <t>/login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,11 +434,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,37 +459,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -491,32 +486,54 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>